<commit_message>
Update - Remove PAR and Add New Sce Files
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_A_SYS_SAD_40TS.xlsx
+++ b/SuppXLS/Scen_A_SYS_SAD_40TS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B8C13B-EE89-405B-BCD6-9E25704ABF6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2844A104-5762-4163-ACC0-F2BAE2288AFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="12" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2988" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="149">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -1426,14 +1426,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>37</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>95249</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9496426" cy="723901"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2025,7 +2025,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2113,13 +2113,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>37</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>176234</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>49</xdr:col>
+      <xdr:col>50</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>29910</xdr:rowOff>
@@ -3961,9 +3961,9 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C857652E-33EB-4E0B-8A21-6A1115888913}" name="rsdsol3" displayName="rsdsol3" ref="B2:AI42" totalsRowShown="0">
-  <autoFilter ref="B2:AI42" xr:uid="{F30D45E5-896D-4C98-9FA5-6590016DF0E8}"/>
-  <tableColumns count="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C857652E-33EB-4E0B-8A21-6A1115888913}" name="rsdsol3" displayName="rsdsol3" ref="B2:AJ42" totalsRowShown="0">
+  <autoFilter ref="B2:AJ42" xr:uid="{F30D45E5-896D-4C98-9FA5-6590016DF0E8}"/>
+  <tableColumns count="35">
     <tableColumn id="1" xr3:uid="{3455E92C-5A81-4C2A-A8F2-C36F90BF4E87}" name="TimeSlice"/>
     <tableColumn id="2" xr3:uid="{BFCC625C-4AC5-4665-82B2-9F6406833EBE}" name="Attribute"/>
     <tableColumn id="3" xr3:uid="{2689E2DD-8B54-408D-BBC7-C5249E764104}" name="Year"/>
@@ -3971,6 +3971,7 @@
     <tableColumn id="5" xr3:uid="{94F31D42-0BD8-40B7-AB15-399A8A9BC81D}" name="Pset_PN"/>
     <tableColumn id="6" xr3:uid="{7E1F1944-CCFC-41D5-AA1E-F5FD7816E31E}" name="Pset_CI"/>
     <tableColumn id="7" xr3:uid="{030406EE-4B75-4D0F-A488-B94815ED0645}" name="IE"/>
+    <tableColumn id="35" xr3:uid="{1A74DC7B-DD05-4DB7-9221-A03981502DDF}" name="Column1"/>
     <tableColumn id="8" xr3:uid="{282E8BB1-82D0-4EC2-AA06-7049BA58C671}" name="National"/>
     <tableColumn id="9" xr3:uid="{2D31AB4B-0F6D-4703-98B1-FA6054208B34}" name="IE-CW"/>
     <tableColumn id="10" xr3:uid="{99601336-A81F-4A5F-B9FD-1EEDFBAD5DF5}" name="IE-KK"/>
@@ -35802,7 +35803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A916DD6D-BEB6-4B16-A1CD-EEF48A0890F6}">
   <dimension ref="B3:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
@@ -44294,10 +44295,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAB2503-B1FF-4F8E-BCAD-738C73A46BF0}">
-  <dimension ref="B1:AI42"/>
+  <dimension ref="B1:AJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44305,12 +44306,12 @@
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -44333,88 +44334,91 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>19</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>21</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>24</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>25</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>26</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>7</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>16</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>18</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>20</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>22</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
@@ -44436,9 +44440,6 @@
       <c r="H3">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I3">
-        <v>5.9999999999999995E-4</v>
-      </c>
       <c r="J3">
         <v>5.9999999999999995E-4</v>
       </c>
@@ -44517,8 +44518,11 @@
       <c r="AI3">
         <v>5.9999999999999995E-4</v>
       </c>
-    </row>
-    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ3">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>33</v>
       </c>
@@ -44540,9 +44544,6 @@
       <c r="H4">
         <v>5.6349999999999997E-2</v>
       </c>
-      <c r="I4">
-        <v>5.6349999999999997E-2</v>
-      </c>
       <c r="J4">
         <v>5.6349999999999997E-2</v>
       </c>
@@ -44621,8 +44622,11 @@
       <c r="AI4">
         <v>5.6349999999999997E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ4">
+        <v>5.6349999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>34</v>
       </c>
@@ -44644,9 +44648,6 @@
       <c r="H5">
         <v>0.23627999999999999</v>
       </c>
-      <c r="I5">
-        <v>0.23627999999999999</v>
-      </c>
       <c r="J5">
         <v>0.23627999999999999</v>
       </c>
@@ -44725,8 +44726,11 @@
       <c r="AI5">
         <v>0.23627999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ5">
+        <v>0.23627999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>35</v>
       </c>
@@ -44748,9 +44752,6 @@
       <c r="H6">
         <v>1.7829999999999999E-2</v>
       </c>
-      <c r="I6">
-        <v>1.7829999999999999E-2</v>
-      </c>
       <c r="J6">
         <v>1.7829999999999999E-2</v>
       </c>
@@ -44829,8 +44830,11 @@
       <c r="AI6">
         <v>1.7829999999999999E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ6">
+        <v>1.7829999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>36</v>
       </c>
@@ -44852,9 +44856,6 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
       <c r="J7">
         <v>0</v>
       </c>
@@ -44933,8 +44934,11 @@
       <c r="AI7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>37</v>
       </c>
@@ -44956,9 +44960,6 @@
       <c r="H8">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="I8">
-        <v>2.9999999999999997E-4</v>
-      </c>
       <c r="J8">
         <v>2.9999999999999997E-4</v>
       </c>
@@ -45037,8 +45038,11 @@
       <c r="AI8">
         <v>2.9999999999999997E-4</v>
       </c>
-    </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ8">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>38</v>
       </c>
@@ -45060,9 +45064,6 @@
       <c r="H9">
         <v>4.7419999999999997E-2</v>
       </c>
-      <c r="I9">
-        <v>4.7419999999999997E-2</v>
-      </c>
       <c r="J9">
         <v>4.7419999999999997E-2</v>
       </c>
@@ -45141,8 +45142,11 @@
       <c r="AI9">
         <v>4.7419999999999997E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ9">
+        <v>4.7419999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>39</v>
       </c>
@@ -45164,9 +45168,6 @@
       <c r="H10">
         <v>0.22863</v>
       </c>
-      <c r="I10">
-        <v>0.22863</v>
-      </c>
       <c r="J10">
         <v>0.22863</v>
       </c>
@@ -45245,8 +45246,11 @@
       <c r="AI10">
         <v>0.22863</v>
       </c>
-    </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ10">
+        <v>0.22863</v>
+      </c>
+    </row>
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>40</v>
       </c>
@@ -45268,9 +45272,6 @@
       <c r="H11">
         <v>1.503E-2</v>
       </c>
-      <c r="I11">
-        <v>1.503E-2</v>
-      </c>
       <c r="J11">
         <v>1.503E-2</v>
       </c>
@@ -45349,8 +45350,11 @@
       <c r="AI11">
         <v>1.503E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ11">
+        <v>1.503E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>41</v>
       </c>
@@ -45372,9 +45376,6 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
       <c r="J12">
         <v>0</v>
       </c>
@@ -45453,8 +45454,11 @@
       <c r="AI12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>42</v>
       </c>
@@ -45476,9 +45480,6 @@
       <c r="H13">
         <v>5.28E-3</v>
       </c>
-      <c r="I13">
-        <v>5.28E-3</v>
-      </c>
       <c r="J13">
         <v>5.28E-3</v>
       </c>
@@ -45557,8 +45558,11 @@
       <c r="AI13">
         <v>5.28E-3</v>
       </c>
-    </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ13">
+        <v>5.28E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>43</v>
       </c>
@@ -45580,9 +45584,6 @@
       <c r="H14">
         <v>0.15382999999999999</v>
       </c>
-      <c r="I14">
-        <v>0.15382999999999999</v>
-      </c>
       <c r="J14">
         <v>0.15382999999999999</v>
       </c>
@@ -45661,8 +45662,11 @@
       <c r="AI14">
         <v>0.15382999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ14">
+        <v>0.15382999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>44</v>
       </c>
@@ -45684,9 +45688,6 @@
       <c r="H15">
         <v>0.3609</v>
       </c>
-      <c r="I15">
-        <v>0.3609</v>
-      </c>
       <c r="J15">
         <v>0.3609</v>
       </c>
@@ -45765,8 +45766,11 @@
       <c r="AI15">
         <v>0.3609</v>
       </c>
-    </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ15">
+        <v>0.3609</v>
+      </c>
+    </row>
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>45</v>
       </c>
@@ -45788,9 +45792,6 @@
       <c r="H16">
         <v>7.6520000000000005E-2</v>
       </c>
-      <c r="I16">
-        <v>7.6520000000000005E-2</v>
-      </c>
       <c r="J16">
         <v>7.6520000000000005E-2</v>
       </c>
@@ -45869,8 +45870,11 @@
       <c r="AI16">
         <v>7.6520000000000005E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ16">
+        <v>7.6520000000000005E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>46</v>
       </c>
@@ -45892,9 +45896,6 @@
       <c r="H17">
         <v>1.23E-3</v>
       </c>
-      <c r="I17">
-        <v>1.23E-3</v>
-      </c>
       <c r="J17">
         <v>1.23E-3</v>
       </c>
@@ -45973,8 +45974,11 @@
       <c r="AI17">
         <v>1.23E-3</v>
       </c>
-    </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ17">
+        <v>1.23E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>47</v>
       </c>
@@ -45996,9 +46000,6 @@
       <c r="H18">
         <v>6.9899999999999997E-3</v>
       </c>
-      <c r="I18">
-        <v>6.9899999999999997E-3</v>
-      </c>
       <c r="J18">
         <v>6.9899999999999997E-3</v>
       </c>
@@ -46077,8 +46078,11 @@
       <c r="AI18">
         <v>6.9899999999999997E-3</v>
       </c>
-    </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ18">
+        <v>6.9899999999999997E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>48</v>
       </c>
@@ -46100,9 +46104,6 @@
       <c r="H19">
         <v>0.15962999999999999</v>
       </c>
-      <c r="I19">
-        <v>0.15962999999999999</v>
-      </c>
       <c r="J19">
         <v>0.15962999999999999</v>
       </c>
@@ -46181,8 +46182,11 @@
       <c r="AI19">
         <v>0.15962999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ19">
+        <v>0.15962999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>49</v>
       </c>
@@ -46204,9 +46208,6 @@
       <c r="H20">
         <v>0.3644</v>
       </c>
-      <c r="I20">
-        <v>0.3644</v>
-      </c>
       <c r="J20">
         <v>0.3644</v>
       </c>
@@ -46285,8 +46286,11 @@
       <c r="AI20">
         <v>0.3644</v>
       </c>
-    </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ20">
+        <v>0.3644</v>
+      </c>
+    </row>
+    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -46308,9 +46312,6 @@
       <c r="H21">
         <v>7.893E-2</v>
       </c>
-      <c r="I21">
-        <v>7.893E-2</v>
-      </c>
       <c r="J21">
         <v>7.893E-2</v>
       </c>
@@ -46389,8 +46390,11 @@
       <c r="AI21">
         <v>7.893E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ21">
+        <v>7.893E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>51</v>
       </c>
@@ -46412,9 +46416,6 @@
       <c r="H22">
         <v>1.57E-3</v>
       </c>
-      <c r="I22">
-        <v>1.57E-3</v>
-      </c>
       <c r="J22">
         <v>1.57E-3</v>
       </c>
@@ -46493,8 +46494,11 @@
       <c r="AI22">
         <v>1.57E-3</v>
       </c>
-    </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ22">
+        <v>1.57E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>52</v>
       </c>
@@ -46516,9 +46520,6 @@
       <c r="H23">
         <v>1.529E-2</v>
       </c>
-      <c r="I23">
-        <v>1.529E-2</v>
-      </c>
       <c r="J23">
         <v>1.529E-2</v>
       </c>
@@ -46597,8 +46598,11 @@
       <c r="AI23">
         <v>1.529E-2</v>
       </c>
-    </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ23">
+        <v>1.529E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>53</v>
       </c>
@@ -46620,9 +46624,6 @@
       <c r="H24">
         <v>0.23</v>
       </c>
-      <c r="I24">
-        <v>0.23</v>
-      </c>
       <c r="J24">
         <v>0.23</v>
       </c>
@@ -46701,8 +46702,11 @@
       <c r="AI24">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ24">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>54</v>
       </c>
@@ -46724,9 +46728,6 @@
       <c r="H25">
         <v>0.42102000000000001</v>
       </c>
-      <c r="I25">
-        <v>0.42102000000000001</v>
-      </c>
       <c r="J25">
         <v>0.42102000000000001</v>
       </c>
@@ -46805,8 +46806,11 @@
       <c r="AI25">
         <v>0.42102000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ25">
+        <v>0.42102000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>55</v>
       </c>
@@ -46828,9 +46832,6 @@
       <c r="H26">
         <v>0.12891</v>
       </c>
-      <c r="I26">
-        <v>0.12891</v>
-      </c>
       <c r="J26">
         <v>0.12891</v>
       </c>
@@ -46909,8 +46910,11 @@
       <c r="AI26">
         <v>0.12891</v>
       </c>
-    </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ26">
+        <v>0.12891</v>
+      </c>
+    </row>
+    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>56</v>
       </c>
@@ -46932,9 +46936,6 @@
       <c r="H27">
         <v>5.1900000000000002E-3</v>
       </c>
-      <c r="I27">
-        <v>5.1900000000000002E-3</v>
-      </c>
       <c r="J27">
         <v>5.1900000000000002E-3</v>
       </c>
@@ -47013,8 +47014,11 @@
       <c r="AI27">
         <v>5.1900000000000002E-3</v>
       </c>
-    </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ27">
+        <v>5.1900000000000002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>57</v>
       </c>
@@ -47036,9 +47040,6 @@
       <c r="H28">
         <v>1.436E-2</v>
       </c>
-      <c r="I28">
-        <v>1.436E-2</v>
-      </c>
       <c r="J28">
         <v>1.436E-2</v>
       </c>
@@ -47117,8 +47118,11 @@
       <c r="AI28">
         <v>1.436E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ28">
+        <v>1.436E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>58</v>
       </c>
@@ -47140,9 +47144,6 @@
       <c r="H29">
         <v>0.22231999999999999</v>
       </c>
-      <c r="I29">
-        <v>0.22231999999999999</v>
-      </c>
       <c r="J29">
         <v>0.22231999999999999</v>
       </c>
@@ -47221,8 +47222,11 @@
       <c r="AI29">
         <v>0.22231999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ29">
+        <v>0.22231999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>59</v>
       </c>
@@ -47244,9 +47248,6 @@
       <c r="H30">
         <v>0.40501999999999999</v>
       </c>
-      <c r="I30">
-        <v>0.40501999999999999</v>
-      </c>
       <c r="J30">
         <v>0.40501999999999999</v>
       </c>
@@ -47325,8 +47326,11 @@
       <c r="AI30">
         <v>0.40501999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ30">
+        <v>0.40501999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>60</v>
       </c>
@@ -47348,9 +47352,6 @@
       <c r="H31">
         <v>0.11814</v>
       </c>
-      <c r="I31">
-        <v>0.11814</v>
-      </c>
       <c r="J31">
         <v>0.11814</v>
       </c>
@@ -47429,8 +47430,11 @@
       <c r="AI31">
         <v>0.11814</v>
       </c>
-    </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ31">
+        <v>0.11814</v>
+      </c>
+    </row>
+    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>61</v>
       </c>
@@ -47452,9 +47456,6 @@
       <c r="H32">
         <v>4.7299999999999998E-3</v>
       </c>
-      <c r="I32">
-        <v>4.7299999999999998E-3</v>
-      </c>
       <c r="J32">
         <v>4.7299999999999998E-3</v>
       </c>
@@ -47533,8 +47534,11 @@
       <c r="AI32">
         <v>4.7299999999999998E-3</v>
       </c>
-    </row>
-    <row r="33" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ32">
+        <v>4.7299999999999998E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>62</v>
       </c>
@@ -47556,9 +47560,6 @@
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
       <c r="J33">
         <v>0</v>
       </c>
@@ -47637,8 +47638,11 @@
       <c r="AI33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>63</v>
       </c>
@@ -47660,9 +47664,6 @@
       <c r="H34">
         <v>6.0299999999999998E-3</v>
       </c>
-      <c r="I34">
-        <v>6.0299999999999998E-3</v>
-      </c>
       <c r="J34">
         <v>6.0299999999999998E-3</v>
       </c>
@@ -47741,8 +47742,11 @@
       <c r="AI34">
         <v>6.0299999999999998E-3</v>
       </c>
-    </row>
-    <row r="35" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ34">
+        <v>6.0299999999999998E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>64</v>
       </c>
@@ -47764,9 +47768,6 @@
       <c r="H35">
         <v>0.11210000000000001</v>
       </c>
-      <c r="I35">
-        <v>0.11210000000000001</v>
-      </c>
       <c r="J35">
         <v>0.11210000000000001</v>
       </c>
@@ -47845,8 +47846,11 @@
       <c r="AI35">
         <v>0.11210000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ35">
+        <v>0.11210000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>65</v>
       </c>
@@ -47868,9 +47872,6 @@
       <c r="H36">
         <v>2.2000000000000001E-4</v>
       </c>
-      <c r="I36">
-        <v>2.2000000000000001E-4</v>
-      </c>
       <c r="J36">
         <v>2.2000000000000001E-4</v>
       </c>
@@ -47949,8 +47950,11 @@
       <c r="AI36">
         <v>2.2000000000000001E-4</v>
       </c>
-    </row>
-    <row r="37" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ36">
+        <v>2.2000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>66</v>
       </c>
@@ -47972,9 +47976,6 @@
       <c r="H37">
         <v>0</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
       <c r="J37">
         <v>0</v>
       </c>
@@ -48053,8 +48054,11 @@
       <c r="AI37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>67</v>
       </c>
@@ -48076,9 +48080,6 @@
       <c r="H38">
         <v>0</v>
       </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
       <c r="J38">
         <v>0</v>
       </c>
@@ -48157,8 +48158,11 @@
       <c r="AI38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>68</v>
       </c>
@@ -48180,9 +48184,6 @@
       <c r="H39">
         <v>6.0499999999999998E-3</v>
       </c>
-      <c r="I39">
-        <v>6.0499999999999998E-3</v>
-      </c>
       <c r="J39">
         <v>6.0499999999999998E-3</v>
       </c>
@@ -48261,8 +48262,11 @@
       <c r="AI39">
         <v>6.0499999999999998E-3</v>
       </c>
-    </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ39">
+        <v>6.0499999999999998E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>69</v>
       </c>
@@ -48284,9 +48288,6 @@
       <c r="H40">
         <v>9.4469999999999998E-2</v>
       </c>
-      <c r="I40">
-        <v>9.4469999999999998E-2</v>
-      </c>
       <c r="J40">
         <v>9.4469999999999998E-2</v>
       </c>
@@ -48365,8 +48366,11 @@
       <c r="AI40">
         <v>9.4469999999999998E-2</v>
       </c>
-    </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ40">
+        <v>9.4469999999999998E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>70</v>
       </c>
@@ -48388,9 +48392,6 @@
       <c r="H41">
         <v>3.8999999999999999E-4</v>
       </c>
-      <c r="I41">
-        <v>3.8999999999999999E-4</v>
-      </c>
       <c r="J41">
         <v>3.8999999999999999E-4</v>
       </c>
@@ -48469,8 +48470,11 @@
       <c r="AI41">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ41">
+        <v>3.8999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>71</v>
       </c>
@@ -48492,9 +48496,6 @@
       <c r="H42">
         <v>0</v>
       </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
       <c r="J42">
         <v>0</v>
       </c>
@@ -48571,6 +48572,9 @@
         <v>0</v>
       </c>
       <c r="AI42">
+        <v>0</v>
+      </c>
+      <c r="AJ42">
         <v>0</v>
       </c>
     </row>
@@ -48589,7 +48593,7 @@
   <dimension ref="B1:AV42"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>